<commit_message>
Add option to set chart font rotation as stacked.
Added the option to allow chart fonts to be rotation to 270 deg
to give a stacked orientation.
</commit_message>
<xml_diff>
--- a/test/regression/xlsx_files/chart_axis26.xlsx
+++ b/test/regression/xlsx_files/chart_axis26.xlsx
@@ -157,18 +157,18 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="73048448"/>
-        <c:axId val="73049984"/>
+        <c:axId val="108315392"/>
+        <c:axId val="108329216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="73048448"/>
+        <c:axId val="108315392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
-          <a:bodyPr rot="2700000"/>
+          <a:bodyPr rot="2700000" vert="horz"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -177,14 +177,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73049984"/>
+        <c:crossAx val="108329216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73049984"/>
+        <c:axId val="108329216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -192,7 +192,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73048448"/>
+        <c:crossAx val="108315392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -205,7 +205,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>

</xml_diff>